<commit_message>
Actualización 7 de junio de 2019
Se actualizó con los exámenes finales de primera ronda.
</commit_message>
<xml_diff>
--- a/MAF-2019-2-Calificaciones.xlsx
+++ b/MAF-2019-2-Calificaciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavo/Documents/Matematicas Avanzadas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D649F036-2AD4-804C-96ED-B25032D62DDF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3672243-69C0-DA4D-8791-66680BB54453}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1540" yWindow="920" windowWidth="38400" windowHeight="21140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Listado de Inscripción " sheetId="1" r:id="rId1"/>
@@ -1543,48 +1543,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1612,6 +1570,48 @@
     <xf numFmtId="9" fontId="9" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2043,46 +2043,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="94" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
+      <c r="A1" s="103" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
+      <c r="F1" s="101"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
+      <c r="I1" s="101"/>
+      <c r="J1" s="101"/>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="89" t="s">
+      <c r="B4" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
       <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
@@ -2093,14 +2093,14 @@
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
+      <c r="C5" s="101"/>
+      <c r="D5" s="101"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
       <c r="H5" s="5" t="s">
         <v>9</v>
       </c>
@@ -2108,49 +2108,49 @@
       <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="92" t="s">
+      <c r="A6" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="90"/>
-      <c r="C6" s="93" t="s">
+      <c r="B6" s="101"/>
+      <c r="C6" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="90"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="90"/>
-      <c r="G6" s="90"/>
+      <c r="D6" s="101"/>
+      <c r="E6" s="101"/>
+      <c r="F6" s="101"/>
+      <c r="G6" s="101"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="92" t="s">
+      <c r="A7" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="90"/>
-      <c r="C7" s="93" t="s">
+      <c r="B7" s="101"/>
+      <c r="C7" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
+      <c r="D7" s="101"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="101"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="92" t="s">
+      <c r="A8" s="100" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="90"/>
-      <c r="C8" s="93" t="s">
+      <c r="B8" s="101"/>
+      <c r="C8" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="90"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="90"/>
+      <c r="D8" s="101"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="101"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -5452,12 +5452,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="94" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
+      <c r="A1" s="103" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
       <c r="E1" s="3"/>
       <c r="F1" s="4"/>
       <c r="G1" s="3"/>
@@ -5466,10 +5466,10 @@
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="6"/>
-      <c r="K1" s="101" t="s">
+      <c r="K1" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="90"/>
+      <c r="L1" s="101"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -5512,12 +5512,12 @@
       <c r="AZ1" s="3"/>
     </row>
     <row r="2" spans="1:53" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
       <c r="E2" s="3"/>
       <c r="F2" s="8"/>
       <c r="G2" s="3"/>
@@ -5692,9 +5692,9 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="100"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="107"/>
+      <c r="G4" s="108"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="4"/>
@@ -5745,55 +5745,55 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="95" t="s">
+      <c r="E5" s="110" t="s">
         <v>190</v>
       </c>
-      <c r="F5" s="96"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="95" t="s">
+      <c r="F5" s="111"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="110" t="s">
         <v>191</v>
       </c>
-      <c r="I5" s="97"/>
-      <c r="J5" s="95" t="s">
+      <c r="I5" s="112"/>
+      <c r="J5" s="110" t="s">
         <v>192</v>
       </c>
-      <c r="K5" s="96"/>
-      <c r="L5" s="96"/>
-      <c r="M5" s="97"/>
-      <c r="N5" s="95" t="s">
+      <c r="K5" s="111"/>
+      <c r="L5" s="111"/>
+      <c r="M5" s="112"/>
+      <c r="N5" s="110" t="s">
         <v>193</v>
       </c>
-      <c r="O5" s="96"/>
-      <c r="P5" s="97"/>
-      <c r="Q5" s="95" t="s">
+      <c r="O5" s="111"/>
+      <c r="P5" s="112"/>
+      <c r="Q5" s="110" t="s">
         <v>194</v>
       </c>
-      <c r="R5" s="96"/>
-      <c r="S5" s="96"/>
-      <c r="T5" s="96"/>
-      <c r="U5" s="96"/>
-      <c r="V5" s="96"/>
-      <c r="W5" s="97"/>
-      <c r="X5" s="91" t="s">
+      <c r="R5" s="111"/>
+      <c r="S5" s="111"/>
+      <c r="T5" s="111"/>
+      <c r="U5" s="111"/>
+      <c r="V5" s="111"/>
+      <c r="W5" s="112"/>
+      <c r="X5" s="105" t="s">
         <v>195</v>
       </c>
-      <c r="Y5" s="90"/>
-      <c r="Z5" s="90"/>
-      <c r="AA5" s="90"/>
-      <c r="AB5" s="91" t="s">
+      <c r="Y5" s="101"/>
+      <c r="Z5" s="101"/>
+      <c r="AA5" s="101"/>
+      <c r="AB5" s="105" t="s">
         <v>196</v>
       </c>
-      <c r="AC5" s="90"/>
-      <c r="AD5" s="90"/>
-      <c r="AE5" s="91" t="s">
+      <c r="AC5" s="101"/>
+      <c r="AD5" s="101"/>
+      <c r="AE5" s="105" t="s">
         <v>197</v>
       </c>
-      <c r="AF5" s="90"/>
-      <c r="AG5" s="91" t="s">
+      <c r="AF5" s="101"/>
+      <c r="AG5" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="AH5" s="90"/>
-      <c r="AI5" s="90"/>
+      <c r="AH5" s="101"/>
+      <c r="AI5" s="101"/>
       <c r="AJ5" s="19" t="s">
         <v>199</v>
       </c>
@@ -14706,6 +14706,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="Q5:W5"/>
+    <mergeCell ref="AG5:AI5"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E4:G4"/>
@@ -14713,12 +14719,6 @@
     <mergeCell ref="J5:M5"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="H5:I5"/>
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="Q5:W5"/>
-    <mergeCell ref="AG5:AI5"/>
-    <mergeCell ref="AB5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -14745,22 +14745,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="94" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
+      <c r="A1" s="103" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16461,7 +16461,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:Y50"/>
+      <selection activeCell="X35" sqref="X35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -16484,23 +16484,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="94" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
+      <c r="A1" s="103" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
       <c r="E2" s="21"/>
       <c r="F2" s="3" t="s">
         <v>203</v>
@@ -16581,42 +16581,42 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="104" t="s">
+      <c r="E6" s="114" t="s">
         <v>205</v>
       </c>
-      <c r="F6" s="105"/>
-      <c r="G6" s="104" t="s">
+      <c r="F6" s="115"/>
+      <c r="G6" s="114" t="s">
         <v>213</v>
       </c>
-      <c r="H6" s="105"/>
-      <c r="I6" s="104" t="s">
+      <c r="H6" s="115"/>
+      <c r="I6" s="114" t="s">
         <v>224</v>
       </c>
-      <c r="J6" s="105"/>
-      <c r="K6" s="107" t="s">
+      <c r="J6" s="115"/>
+      <c r="K6" s="116" t="s">
         <v>229</v>
       </c>
-      <c r="L6" s="105"/>
-      <c r="M6" s="107" t="s">
+      <c r="L6" s="115"/>
+      <c r="M6" s="116" t="s">
         <v>234</v>
       </c>
-      <c r="N6" s="105"/>
-      <c r="O6" s="107" t="s">
+      <c r="N6" s="115"/>
+      <c r="O6" s="116" t="s">
         <v>235</v>
       </c>
-      <c r="P6" s="105"/>
-      <c r="Q6" s="107" t="s">
+      <c r="P6" s="115"/>
+      <c r="Q6" s="116" t="s">
         <v>236</v>
       </c>
-      <c r="R6" s="105"/>
-      <c r="S6" s="107" t="s">
+      <c r="R6" s="115"/>
+      <c r="S6" s="116" t="s">
         <v>237</v>
       </c>
-      <c r="T6" s="105"/>
-      <c r="U6" s="108" t="s">
+      <c r="T6" s="115"/>
+      <c r="U6" s="113" t="s">
         <v>240</v>
       </c>
-      <c r="V6" s="97"/>
+      <c r="V6" s="112"/>
       <c r="W6" s="28" t="s">
         <v>255</v>
       </c>
@@ -16632,38 +16632,38 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="102" t="s">
+      <c r="E7" s="118" t="s">
         <v>258</v>
       </c>
-      <c r="F7" s="103"/>
-      <c r="G7" s="102" t="s">
+      <c r="F7" s="119"/>
+      <c r="G7" s="118" t="s">
         <v>259</v>
       </c>
-      <c r="H7" s="103"/>
-      <c r="I7" s="102" t="s">
+      <c r="H7" s="119"/>
+      <c r="I7" s="118" t="s">
         <v>260</v>
       </c>
-      <c r="J7" s="103"/>
-      <c r="K7" s="102" t="s">
+      <c r="J7" s="119"/>
+      <c r="K7" s="118" t="s">
         <v>261</v>
       </c>
-      <c r="L7" s="103"/>
-      <c r="M7" s="106" t="s">
+      <c r="L7" s="119"/>
+      <c r="M7" s="117" t="s">
         <v>262</v>
       </c>
-      <c r="N7" s="105"/>
-      <c r="O7" s="106" t="s">
+      <c r="N7" s="115"/>
+      <c r="O7" s="117" t="s">
         <v>263</v>
       </c>
-      <c r="P7" s="105"/>
-      <c r="Q7" s="106" t="s">
+      <c r="P7" s="115"/>
+      <c r="Q7" s="117" t="s">
         <v>264</v>
       </c>
-      <c r="R7" s="105"/>
-      <c r="S7" s="106" t="s">
+      <c r="R7" s="115"/>
+      <c r="S7" s="117" t="s">
         <v>265</v>
       </c>
-      <c r="T7" s="105"/>
+      <c r="T7" s="115"/>
       <c r="U7" s="33" t="s">
         <v>266</v>
       </c>
@@ -18260,12 +18260,13 @@
       <c r="W35" s="53">
         <v>0.78064516129032258</v>
       </c>
-      <c r="X35" s="68">
-        <v>4.8</v>
+      <c r="X35" s="54">
+        <f t="shared" ref="X35" si="8">U35+W35</f>
+        <v>3.6229308755760368</v>
       </c>
       <c r="Y35" s="65">
         <f>X35+1.7</f>
-        <v>6.5</v>
+        <v>5.3229308755760369</v>
       </c>
     </row>
     <row r="36" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -18680,7 +18681,7 @@
       <c r="S43" s="66"/>
       <c r="T43" s="82"/>
       <c r="U43" s="52">
-        <f t="shared" ref="U43:U45" si="8">(SUM(F43,H43,J43,L43,(N43+P43)/2,R43,T43)/7)*0.6</f>
+        <f t="shared" ref="U43:U45" si="9">(SUM(F43,H43,J43,L43,(N43+P43)/2,R43,T43)/7)*0.6</f>
         <v>2.4964285714285719</v>
       </c>
       <c r="V43" s="45"/>
@@ -18688,7 +18689,7 @@
         <v>1.5393548387096774</v>
       </c>
       <c r="X43" s="54">
-        <f t="shared" ref="X43:X45" si="9">U43+W43</f>
+        <f t="shared" ref="X43:X45" si="10">U43+W43</f>
         <v>4.035783410138249</v>
       </c>
       <c r="Y43" s="33">
@@ -18757,7 +18758,7 @@
         <v>10</v>
       </c>
       <c r="U44" s="52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>4.298571428571428</v>
       </c>
       <c r="V44" s="45"/>
@@ -18765,7 +18766,7 @@
         <v>2.3780645161290326</v>
       </c>
       <c r="X44" s="54">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.6766359447004611</v>
       </c>
       <c r="Y44" s="33">
@@ -18834,7 +18835,7 @@
         <v>3.33</v>
       </c>
       <c r="U45" s="52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.0871428571428572</v>
       </c>
       <c r="V45" s="45"/>
@@ -18842,7 +18843,7 @@
         <v>2.4774193548387098</v>
       </c>
       <c r="X45" s="54">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4.564562211981567</v>
       </c>
       <c r="Y45" s="56">
@@ -21955,12 +21956,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="O6:P6"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="O7:P7"/>
@@ -21974,6 +21969,12 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G7:H7"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="O6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -21985,2071 +21986,2071 @@
   <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="110" t="s">
+      <c r="B1" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="110" t="s">
+      <c r="C1" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="116" t="s">
+      <c r="D1" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="110" t="s">
+      <c r="E1" s="90" t="s">
         <v>272</v>
       </c>
-      <c r="F1" s="110" t="s">
+      <c r="F1" s="90" t="s">
         <v>273</v>
       </c>
-      <c r="G1" s="110" t="s">
+      <c r="G1" s="90" t="s">
         <v>274</v>
       </c>
-      <c r="H1" s="110" t="s">
+      <c r="H1" s="90" t="s">
         <v>275</v>
       </c>
-      <c r="I1" s="110" t="s">
+      <c r="I1" s="90" t="s">
         <v>276</v>
       </c>
-      <c r="J1" s="110" t="s">
+      <c r="J1" s="90" t="s">
         <v>277</v>
       </c>
-      <c r="K1" s="110" t="s">
+      <c r="K1" s="90" t="s">
         <v>278</v>
       </c>
-      <c r="L1" s="110" t="s">
+      <c r="L1" s="90" t="s">
         <v>279</v>
       </c>
-      <c r="M1" s="110" t="s">
+      <c r="M1" s="90" t="s">
         <v>280</v>
       </c>
-      <c r="N1" s="118" t="s">
+      <c r="N1" s="98" t="s">
         <v>284</v>
       </c>
-      <c r="O1" s="118" t="s">
+      <c r="O1" s="98" t="s">
         <v>285</v>
       </c>
-      <c r="P1" s="110" t="s">
+      <c r="P1" s="90" t="s">
         <v>281</v>
       </c>
-      <c r="Q1" s="110" t="s">
+      <c r="Q1" s="90" t="s">
         <v>282</v>
       </c>
-      <c r="R1" s="110" t="s">
+      <c r="R1" s="90" t="s">
         <v>257</v>
       </c>
-      <c r="S1" s="113" t="s">
+      <c r="S1" s="93" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="109" t="s">
+      <c r="B2" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="109" t="s">
+      <c r="C2" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="117">
+      <c r="D2" s="97">
         <v>314002411</v>
       </c>
-      <c r="E2" s="110">
+      <c r="E2" s="90">
         <v>4.4000000000000004</v>
       </c>
-      <c r="F2" s="110">
+      <c r="F2" s="90">
         <v>3.82</v>
       </c>
-      <c r="G2" s="110">
+      <c r="G2" s="90">
         <v>4.5999999999999996</v>
       </c>
-      <c r="H2" s="110">
+      <c r="H2" s="90">
         <v>8.77</v>
       </c>
-      <c r="I2" s="110">
+      <c r="I2" s="90">
         <v>5.6</v>
       </c>
-      <c r="J2" s="110">
+      <c r="J2" s="90">
         <v>4.67</v>
       </c>
-      <c r="K2" s="110">
+      <c r="K2" s="90">
         <v>5</v>
       </c>
-      <c r="L2" s="110">
+      <c r="L2" s="90">
         <v>5.83</v>
       </c>
-      <c r="M2" s="111">
+      <c r="M2" s="91">
         <v>3.2189999999999999</v>
       </c>
-      <c r="N2" s="118">
+      <c r="N2" s="98">
         <v>13</v>
       </c>
-      <c r="O2" s="119">
+      <c r="O2" s="99">
         <v>0.42</v>
       </c>
-      <c r="P2" s="111">
+      <c r="P2" s="91">
         <v>1.3548387096774195</v>
       </c>
-      <c r="Q2" s="111">
+      <c r="Q2" s="91">
         <v>4.5738387096774193</v>
       </c>
-      <c r="R2" s="111" t="s">
+      <c r="R2" s="91" t="s">
         <v>282</v>
       </c>
-      <c r="S2" s="114">
+      <c r="S2" s="94">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A3" s="109" t="s">
+      <c r="A3" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="109" t="s">
+      <c r="B3" s="89" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="109" t="s">
+      <c r="C3" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="117">
+      <c r="D3" s="97">
         <v>312090762</v>
       </c>
-      <c r="E3" s="110">
+      <c r="E3" s="90">
         <v>1.96</v>
       </c>
-      <c r="F3" s="110">
+      <c r="F3" s="90">
         <v>1.36</v>
       </c>
-      <c r="G3" s="110">
+      <c r="G3" s="90">
         <v>9.1</v>
       </c>
-      <c r="H3" s="110">
+      <c r="H3" s="90">
         <v>10</v>
       </c>
-      <c r="I3" s="110">
+      <c r="I3" s="90">
         <v>2.8</v>
       </c>
-      <c r="J3" s="110">
+      <c r="J3" s="90">
         <v>9.1</v>
       </c>
-      <c r="K3" s="110">
+      <c r="K3" s="90">
         <v>8</v>
       </c>
-      <c r="L3" s="110">
+      <c r="L3" s="90">
         <v>10</v>
       </c>
-      <c r="M3" s="111">
+      <c r="M3" s="91">
         <v>3.9745714285714286</v>
       </c>
-      <c r="N3" s="118">
+      <c r="N3" s="98">
         <v>24</v>
       </c>
-      <c r="O3" s="119">
+      <c r="O3" s="99">
         <v>0.77</v>
       </c>
-      <c r="P3" s="111">
+      <c r="P3" s="91">
         <v>2.8683870967741938</v>
       </c>
-      <c r="Q3" s="111">
+      <c r="Q3" s="91">
         <v>6.8429585253456224</v>
       </c>
-      <c r="R3" s="112">
+      <c r="R3" s="92">
         <v>9</v>
       </c>
-      <c r="S3" s="114">
+      <c r="S3" s="94">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A4" s="109" t="s">
+      <c r="A4" s="89" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="109" t="s">
+      <c r="B4" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="109" t="s">
+      <c r="C4" s="89" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="117">
+      <c r="D4" s="97">
         <v>310047564</v>
       </c>
-      <c r="E4" s="110">
+      <c r="E4" s="90">
         <v>3.33</v>
       </c>
-      <c r="F4" s="110">
+      <c r="F4" s="90">
         <v>3.25</v>
       </c>
-      <c r="G4" s="110">
+      <c r="G4" s="90">
         <v>2.66</v>
       </c>
-      <c r="H4" s="110">
+      <c r="H4" s="90">
         <v>1.5</v>
       </c>
-      <c r="I4" s="110"/>
-      <c r="J4" s="110"/>
-      <c r="K4" s="110"/>
-      <c r="L4" s="110"/>
-      <c r="M4" s="111"/>
-      <c r="N4" s="118">
+      <c r="I4" s="90"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="98">
         <v>4</v>
       </c>
-      <c r="O4" s="119">
+      <c r="O4" s="99">
         <v>0.13</v>
       </c>
-      <c r="P4" s="111">
+      <c r="P4" s="91">
         <v>0.32258064516129031</v>
       </c>
-      <c r="Q4" s="111">
+      <c r="Q4" s="91">
         <v>5</v>
       </c>
-      <c r="R4" s="112">
+      <c r="R4" s="92">
         <v>5</v>
       </c>
-      <c r="S4" s="109"/>
+      <c r="S4" s="89"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A5" s="109" t="s">
+      <c r="A5" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="109" t="s">
+      <c r="B5" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="109" t="s">
+      <c r="C5" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="117">
+      <c r="D5" s="97">
         <v>310114303</v>
       </c>
-      <c r="E5" s="110"/>
-      <c r="F5" s="110"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="110"/>
-      <c r="I5" s="110"/>
-      <c r="J5" s="110"/>
-      <c r="K5" s="110"/>
-      <c r="L5" s="110"/>
-      <c r="M5" s="111"/>
-      <c r="N5" s="118">
-        <v>0</v>
-      </c>
-      <c r="O5" s="119">
-        <v>0</v>
-      </c>
-      <c r="P5" s="111">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="111" t="s">
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90"/>
+      <c r="J5" s="90"/>
+      <c r="K5" s="90"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="98">
+        <v>0</v>
+      </c>
+      <c r="O5" s="99">
+        <v>0</v>
+      </c>
+      <c r="P5" s="91">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R5" s="112">
+      <c r="R5" s="92">
         <v>5</v>
       </c>
-      <c r="S5" s="109"/>
+      <c r="S5" s="89"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="109" t="s">
+      <c r="B6" s="89" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="109" t="s">
+      <c r="C6" s="89" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="117">
+      <c r="D6" s="97">
         <v>313178683</v>
       </c>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="110"/>
-      <c r="K6" s="110"/>
-      <c r="L6" s="110"/>
-      <c r="M6" s="111"/>
-      <c r="N6" s="118">
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="90"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="90"/>
+      <c r="K6" s="90"/>
+      <c r="L6" s="90"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="98">
         <v>3</v>
       </c>
-      <c r="O6" s="119">
+      <c r="O6" s="99">
         <v>0.1</v>
       </c>
-      <c r="P6" s="111">
+      <c r="P6" s="91">
         <v>0.34838709677419355</v>
       </c>
-      <c r="Q6" s="111">
+      <c r="Q6" s="91">
         <v>5</v>
       </c>
-      <c r="R6" s="112">
+      <c r="R6" s="92">
         <v>5</v>
       </c>
-      <c r="S6" s="109"/>
+      <c r="S6" s="89"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A7" s="109" t="s">
+      <c r="A7" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="109" t="s">
+      <c r="B7" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="109" t="s">
+      <c r="C7" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="117">
+      <c r="D7" s="97">
         <v>311257667</v>
       </c>
-      <c r="E7" s="110">
+      <c r="E7" s="90">
         <v>1.83</v>
       </c>
-      <c r="F7" s="110">
+      <c r="F7" s="90">
         <v>2.9</v>
       </c>
-      <c r="G7" s="110">
+      <c r="G7" s="90">
         <v>4.95</v>
       </c>
-      <c r="H7" s="110">
+      <c r="H7" s="90">
         <v>6.44</v>
       </c>
-      <c r="I7" s="110">
+      <c r="I7" s="90">
         <v>0.4</v>
       </c>
-      <c r="J7" s="110">
+      <c r="J7" s="90">
         <v>8.83</v>
       </c>
-      <c r="K7" s="110">
+      <c r="K7" s="90">
         <v>8.32</v>
       </c>
-      <c r="L7" s="110">
+      <c r="L7" s="90">
         <v>8.8000000000000007</v>
       </c>
-      <c r="M7" s="111">
+      <c r="M7" s="91">
         <v>3.2447142857142861</v>
       </c>
-      <c r="N7" s="118">
+      <c r="N7" s="98">
         <v>12</v>
       </c>
-      <c r="O7" s="119">
+      <c r="O7" s="99">
         <v>0.39</v>
       </c>
-      <c r="P7" s="111">
+      <c r="P7" s="91">
         <v>1.3548387096774195</v>
       </c>
-      <c r="Q7" s="111">
+      <c r="Q7" s="91">
         <v>4.599552995391706</v>
       </c>
-      <c r="R7" s="112" t="s">
+      <c r="R7" s="92" t="s">
         <v>282</v>
       </c>
-      <c r="S7" s="114">
+      <c r="S7" s="94">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A8" s="109" t="s">
+      <c r="A8" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="109" t="s">
+      <c r="B8" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="109" t="s">
+      <c r="C8" s="89" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="117">
+      <c r="D8" s="97">
         <v>312355436</v>
       </c>
-      <c r="E8" s="110">
+      <c r="E8" s="90">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F8" s="110">
+      <c r="F8" s="90">
         <v>2.75</v>
       </c>
-      <c r="G8" s="110"/>
-      <c r="H8" s="110"/>
-      <c r="I8" s="110"/>
-      <c r="J8" s="110"/>
-      <c r="K8" s="110"/>
-      <c r="L8" s="110"/>
-      <c r="M8" s="111"/>
-      <c r="N8" s="118">
+      <c r="G8" s="90"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="91"/>
+      <c r="N8" s="98">
         <v>2</v>
       </c>
-      <c r="O8" s="119">
+      <c r="O8" s="99">
         <v>0.06</v>
       </c>
-      <c r="P8" s="111">
+      <c r="P8" s="91">
         <v>0.18064516129032257</v>
       </c>
-      <c r="Q8" s="111">
+      <c r="Q8" s="91">
         <v>5</v>
       </c>
-      <c r="R8" s="112">
+      <c r="R8" s="92">
         <v>5</v>
       </c>
-      <c r="S8" s="115"/>
+      <c r="S8" s="95"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A9" s="109" t="s">
+      <c r="A9" s="89" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="109" t="s">
+      <c r="B9" s="89" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="109" t="s">
+      <c r="C9" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="117">
+      <c r="D9" s="97">
         <v>314082381</v>
       </c>
-      <c r="E9" s="110">
+      <c r="E9" s="90">
         <v>5.48</v>
       </c>
-      <c r="F9" s="110">
+      <c r="F9" s="90">
         <v>5</v>
       </c>
-      <c r="G9" s="110"/>
-      <c r="H9" s="110"/>
-      <c r="I9" s="110"/>
-      <c r="J9" s="110"/>
-      <c r="K9" s="110"/>
-      <c r="L9" s="110"/>
-      <c r="M9" s="111"/>
-      <c r="N9" s="118">
+      <c r="G9" s="90"/>
+      <c r="H9" s="90"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="91"/>
+      <c r="N9" s="98">
         <v>7</v>
       </c>
-      <c r="O9" s="119">
+      <c r="O9" s="99">
         <v>0.23</v>
       </c>
-      <c r="P9" s="111">
+      <c r="P9" s="91">
         <v>0.76129032258064511</v>
       </c>
-      <c r="Q9" s="111">
+      <c r="Q9" s="91">
         <v>5</v>
       </c>
-      <c r="R9" s="112">
+      <c r="R9" s="92">
         <v>5</v>
       </c>
-      <c r="S9" s="115"/>
+      <c r="S9" s="95"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A10" s="109" t="s">
+      <c r="A10" s="89" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="109" t="s">
+      <c r="B10" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="109" t="s">
+      <c r="C10" s="89" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="117">
+      <c r="D10" s="97">
         <v>411048141</v>
       </c>
-      <c r="E10" s="110"/>
-      <c r="F10" s="110"/>
-      <c r="G10" s="110"/>
-      <c r="H10" s="110"/>
-      <c r="I10" s="110"/>
-      <c r="J10" s="110"/>
-      <c r="K10" s="110"/>
-      <c r="L10" s="110"/>
-      <c r="M10" s="111"/>
-      <c r="N10" s="118">
-        <v>0</v>
-      </c>
-      <c r="O10" s="119">
-        <v>0</v>
-      </c>
-      <c r="P10" s="111">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="111" t="s">
+      <c r="E10" s="90"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="90"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="90"/>
+      <c r="J10" s="90"/>
+      <c r="K10" s="90"/>
+      <c r="L10" s="90"/>
+      <c r="M10" s="91"/>
+      <c r="N10" s="98">
+        <v>0</v>
+      </c>
+      <c r="O10" s="99">
+        <v>0</v>
+      </c>
+      <c r="P10" s="91">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R10" s="112" t="s">
+      <c r="R10" s="92" t="s">
         <v>271</v>
       </c>
-      <c r="S10" s="115"/>
+      <c r="S10" s="95"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A11" s="109" t="s">
+      <c r="A11" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="109" t="s">
+      <c r="B11" s="89" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="109" t="s">
+      <c r="C11" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="117">
+      <c r="D11" s="97">
         <v>313023837</v>
       </c>
-      <c r="E11" s="110"/>
-      <c r="F11" s="110"/>
-      <c r="G11" s="110"/>
-      <c r="H11" s="110"/>
-      <c r="I11" s="110"/>
-      <c r="J11" s="110"/>
-      <c r="K11" s="110"/>
-      <c r="L11" s="110"/>
-      <c r="M11" s="111"/>
-      <c r="N11" s="118">
-        <v>0</v>
-      </c>
-      <c r="O11" s="119">
-        <v>0</v>
-      </c>
-      <c r="P11" s="111">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="111" t="s">
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="90"/>
+      <c r="I11" s="90"/>
+      <c r="J11" s="90"/>
+      <c r="K11" s="90"/>
+      <c r="L11" s="90"/>
+      <c r="M11" s="91"/>
+      <c r="N11" s="98">
+        <v>0</v>
+      </c>
+      <c r="O11" s="99">
+        <v>0</v>
+      </c>
+      <c r="P11" s="91">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R11" s="112" t="s">
+      <c r="R11" s="92" t="s">
         <v>271</v>
       </c>
-      <c r="S11" s="115"/>
+      <c r="S11" s="95"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A12" s="109" t="s">
+      <c r="A12" s="89" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="109" t="s">
+      <c r="B12" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="109" t="s">
+      <c r="C12" s="89" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="117">
+      <c r="D12" s="97">
         <v>313535327</v>
       </c>
-      <c r="E12" s="110">
+      <c r="E12" s="90">
         <v>1.66</v>
       </c>
-      <c r="F12" s="110">
+      <c r="F12" s="90">
         <v>2.72</v>
       </c>
-      <c r="G12" s="110">
+      <c r="G12" s="90">
         <v>7.6</v>
       </c>
-      <c r="H12" s="110">
+      <c r="H12" s="90">
         <v>6.61</v>
       </c>
-      <c r="I12" s="110"/>
-      <c r="J12" s="110"/>
-      <c r="K12" s="110"/>
-      <c r="L12" s="110"/>
-      <c r="M12" s="111"/>
-      <c r="N12" s="118">
+      <c r="I12" s="90"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="90"/>
+      <c r="L12" s="90"/>
+      <c r="M12" s="91"/>
+      <c r="N12" s="98">
         <v>8</v>
       </c>
-      <c r="O12" s="119">
+      <c r="O12" s="99">
         <v>0.26</v>
       </c>
-      <c r="P12" s="111">
+      <c r="P12" s="91">
         <v>0.82580645161290323</v>
       </c>
-      <c r="Q12" s="111">
+      <c r="Q12" s="91">
         <v>5</v>
       </c>
-      <c r="R12" s="112">
+      <c r="R12" s="92">
         <v>5</v>
       </c>
-      <c r="S12" s="115"/>
+      <c r="S12" s="95"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A13" s="109" t="s">
+      <c r="A13" s="89" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="109" t="s">
+      <c r="B13" s="89" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="109" t="s">
+      <c r="C13" s="89" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="117">
+      <c r="D13" s="97">
         <v>309110518</v>
       </c>
-      <c r="E13" s="110"/>
-      <c r="F13" s="110"/>
-      <c r="G13" s="110"/>
-      <c r="H13" s="110"/>
-      <c r="I13" s="110"/>
-      <c r="J13" s="110"/>
-      <c r="K13" s="110"/>
-      <c r="L13" s="110"/>
-      <c r="M13" s="111"/>
-      <c r="N13" s="118">
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="90"/>
+      <c r="I13" s="90"/>
+      <c r="J13" s="90"/>
+      <c r="K13" s="90"/>
+      <c r="L13" s="90"/>
+      <c r="M13" s="91"/>
+      <c r="N13" s="98">
         <v>3</v>
       </c>
-      <c r="O13" s="119">
+      <c r="O13" s="99">
         <v>0.1</v>
       </c>
-      <c r="P13" s="111">
+      <c r="P13" s="91">
         <v>0.24903225806451612</v>
       </c>
-      <c r="Q13" s="111" t="s">
+      <c r="Q13" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R13" s="112">
+      <c r="R13" s="92">
         <v>5</v>
       </c>
-      <c r="S13" s="115"/>
+      <c r="S13" s="95"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A14" s="109" t="s">
+      <c r="A14" s="89" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="109" t="s">
+      <c r="B14" s="89" t="s">
         <v>77</v>
       </c>
-      <c r="C14" s="109" t="s">
+      <c r="C14" s="89" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="117">
+      <c r="D14" s="97">
         <v>310009322</v>
       </c>
-      <c r="E14" s="110">
+      <c r="E14" s="90">
         <v>4</v>
       </c>
-      <c r="F14" s="110">
+      <c r="F14" s="90">
         <v>6.3</v>
       </c>
-      <c r="G14" s="110">
+      <c r="G14" s="90">
         <v>5.75</v>
       </c>
-      <c r="H14" s="110">
+      <c r="H14" s="90">
         <v>7.05</v>
       </c>
-      <c r="I14" s="110">
+      <c r="I14" s="90">
         <v>5</v>
       </c>
-      <c r="J14" s="110">
+      <c r="J14" s="90">
         <v>6.66</v>
       </c>
-      <c r="K14" s="110">
+      <c r="K14" s="90">
         <v>3.75</v>
       </c>
-      <c r="L14" s="110">
+      <c r="L14" s="90">
         <v>4.8</v>
       </c>
-      <c r="M14" s="111">
+      <c r="M14" s="91">
         <v>3.2125714285714282</v>
       </c>
-      <c r="N14" s="118">
+      <c r="N14" s="98">
         <v>12</v>
       </c>
-      <c r="O14" s="119">
+      <c r="O14" s="99">
         <v>0.39</v>
       </c>
-      <c r="P14" s="111">
+      <c r="P14" s="91">
         <v>1.1225806451612903</v>
       </c>
-      <c r="Q14" s="111">
+      <c r="Q14" s="91">
         <v>4.3351520737327185</v>
       </c>
-      <c r="R14" s="112" t="s">
+      <c r="R14" s="92" t="s">
         <v>282</v>
       </c>
-      <c r="S14" s="114">
+      <c r="S14" s="94">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A15" s="109" t="s">
+      <c r="A15" s="89" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="109" t="s">
+      <c r="B15" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="109" t="s">
+      <c r="C15" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="D15" s="117">
+      <c r="D15" s="97">
         <v>312053613</v>
       </c>
-      <c r="E15" s="110">
+      <c r="E15" s="90">
         <v>7.05</v>
       </c>
-      <c r="F15" s="110">
+      <c r="F15" s="90">
         <v>5.6</v>
       </c>
-      <c r="G15" s="110">
+      <c r="G15" s="90">
         <v>4.7</v>
       </c>
-      <c r="H15" s="110">
+      <c r="H15" s="90">
         <v>8.2200000000000006</v>
       </c>
-      <c r="I15" s="110">
+      <c r="I15" s="90">
         <v>4.4000000000000004</v>
       </c>
-      <c r="J15" s="110">
+      <c r="J15" s="90">
         <v>7.5</v>
       </c>
-      <c r="K15" s="110">
+      <c r="K15" s="90">
         <v>7.5</v>
       </c>
-      <c r="L15" s="110">
+      <c r="L15" s="90">
         <v>8</v>
       </c>
-      <c r="M15" s="111">
+      <c r="M15" s="91">
         <v>4.0302857142857134</v>
       </c>
-      <c r="N15" s="118">
+      <c r="N15" s="98">
         <v>15</v>
       </c>
-      <c r="O15" s="119">
+      <c r="O15" s="99">
         <v>0.48</v>
       </c>
-      <c r="P15" s="111">
+      <c r="P15" s="91">
         <v>1.7677419354838708</v>
       </c>
-      <c r="Q15" s="111">
+      <c r="Q15" s="91">
         <v>5.7980276497695842</v>
       </c>
-      <c r="R15" s="112">
+      <c r="R15" s="92">
         <v>7</v>
       </c>
-      <c r="S15" s="114">
+      <c r="S15" s="94">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A16" s="109" t="s">
+      <c r="A16" s="89" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="109" t="s">
+      <c r="B16" s="89" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="109" t="s">
+      <c r="C16" s="89" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="117">
+      <c r="D16" s="97">
         <v>307039459</v>
       </c>
-      <c r="E16" s="110"/>
-      <c r="F16" s="110"/>
-      <c r="G16" s="110"/>
-      <c r="H16" s="110"/>
-      <c r="I16" s="110"/>
-      <c r="J16" s="110"/>
-      <c r="K16" s="110"/>
-      <c r="L16" s="110"/>
-      <c r="M16" s="111"/>
-      <c r="N16" s="118">
-        <v>0</v>
-      </c>
-      <c r="O16" s="119">
-        <v>0</v>
-      </c>
-      <c r="P16" s="111">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="111" t="s">
+      <c r="E16" s="90"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="90"/>
+      <c r="I16" s="90"/>
+      <c r="J16" s="90"/>
+      <c r="K16" s="90"/>
+      <c r="L16" s="90"/>
+      <c r="M16" s="91"/>
+      <c r="N16" s="98">
+        <v>0</v>
+      </c>
+      <c r="O16" s="99">
+        <v>0</v>
+      </c>
+      <c r="P16" s="91">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R16" s="112" t="s">
+      <c r="R16" s="92" t="s">
         <v>271</v>
       </c>
-      <c r="S16" s="115"/>
+      <c r="S16" s="95"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A17" s="109" t="s">
+      <c r="A17" s="89" t="s">
         <v>89</v>
       </c>
-      <c r="B17" s="109" t="s">
+      <c r="B17" s="89" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="109" t="s">
+      <c r="C17" s="89" t="s">
         <v>91</v>
       </c>
-      <c r="D17" s="117">
+      <c r="D17" s="97">
         <v>312247485</v>
       </c>
-      <c r="E17" s="110">
+      <c r="E17" s="90">
         <v>8.5</v>
       </c>
-      <c r="F17" s="110">
+      <c r="F17" s="90">
         <v>7.86</v>
       </c>
-      <c r="G17" s="110">
+      <c r="G17" s="90">
         <v>8.6999999999999993</v>
       </c>
-      <c r="H17" s="110">
+      <c r="H17" s="90">
         <v>9.5</v>
       </c>
-      <c r="I17" s="110">
+      <c r="I17" s="90">
         <v>5.6</v>
       </c>
-      <c r="J17" s="110">
+      <c r="J17" s="90">
         <v>8.33</v>
       </c>
-      <c r="K17" s="110">
+      <c r="K17" s="90">
         <v>8.75</v>
       </c>
-      <c r="L17" s="110">
+      <c r="L17" s="90">
         <v>8</v>
       </c>
-      <c r="M17" s="111">
+      <c r="M17" s="91">
         <v>4.9950000000000001</v>
       </c>
-      <c r="N17" s="118">
+      <c r="N17" s="98">
         <v>17</v>
       </c>
-      <c r="O17" s="119">
+      <c r="O17" s="99">
         <v>0.55000000000000004</v>
       </c>
-      <c r="P17" s="111">
+      <c r="P17" s="91">
         <v>2.0774193548387099</v>
       </c>
-      <c r="Q17" s="111">
+      <c r="Q17" s="91">
         <v>7.0724193548387095</v>
       </c>
-      <c r="R17" s="112">
+      <c r="R17" s="92">
         <v>9</v>
       </c>
-      <c r="S17" s="114">
+      <c r="S17" s="94">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A18" s="109" t="s">
+      <c r="A18" s="89" t="s">
         <v>89</v>
       </c>
-      <c r="B18" s="109" t="s">
+      <c r="B18" s="89" t="s">
         <v>93</v>
       </c>
-      <c r="C18" s="109" t="s">
+      <c r="C18" s="89" t="s">
         <v>94</v>
       </c>
-      <c r="D18" s="117">
+      <c r="D18" s="97">
         <v>310019040</v>
       </c>
-      <c r="E18" s="110">
+      <c r="E18" s="90">
         <v>3.23</v>
       </c>
-      <c r="F18" s="110">
+      <c r="F18" s="90">
         <v>6.9</v>
       </c>
-      <c r="G18" s="110"/>
-      <c r="H18" s="110"/>
-      <c r="I18" s="110"/>
-      <c r="J18" s="110"/>
-      <c r="K18" s="110"/>
-      <c r="L18" s="110"/>
-      <c r="M18" s="111"/>
-      <c r="N18" s="118">
+      <c r="G18" s="90"/>
+      <c r="H18" s="90"/>
+      <c r="I18" s="90"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="90"/>
+      <c r="L18" s="90"/>
+      <c r="M18" s="91"/>
+      <c r="N18" s="98">
         <v>2</v>
       </c>
-      <c r="O18" s="119">
+      <c r="O18" s="99">
         <v>0.06</v>
       </c>
-      <c r="P18" s="111">
+      <c r="P18" s="91">
         <v>0.16774193548387098</v>
       </c>
-      <c r="Q18" s="111">
+      <c r="Q18" s="91">
         <v>5</v>
       </c>
-      <c r="R18" s="112">
+      <c r="R18" s="92">
         <v>5</v>
       </c>
-      <c r="S18" s="115"/>
+      <c r="S18" s="95"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A19" s="109" t="s">
+      <c r="A19" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="B19" s="109" t="s">
+      <c r="B19" s="89" t="s">
         <v>97</v>
       </c>
-      <c r="C19" s="109" t="s">
+      <c r="C19" s="89" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="117">
+      <c r="D19" s="97">
         <v>313265693</v>
       </c>
-      <c r="E19" s="110">
+      <c r="E19" s="90">
         <v>9.8000000000000007</v>
       </c>
-      <c r="F19" s="110">
+      <c r="F19" s="90">
         <v>8.66</v>
       </c>
-      <c r="G19" s="110">
+      <c r="G19" s="90">
         <v>7.28</v>
       </c>
-      <c r="H19" s="110">
+      <c r="H19" s="90">
         <v>6.61</v>
       </c>
-      <c r="I19" s="110">
+      <c r="I19" s="90">
         <v>3.6</v>
       </c>
-      <c r="J19" s="110">
+      <c r="J19" s="90">
         <v>4.5</v>
       </c>
-      <c r="K19" s="110">
+      <c r="K19" s="90">
         <v>5.12</v>
       </c>
-      <c r="L19" s="110">
+      <c r="L19" s="90">
         <v>7.08</v>
       </c>
-      <c r="M19" s="111">
+      <c r="M19" s="91">
         <v>4.1657142857142855</v>
       </c>
-      <c r="N19" s="118">
+      <c r="N19" s="98">
         <v>19</v>
       </c>
-      <c r="O19" s="119">
+      <c r="O19" s="99">
         <v>0.61</v>
       </c>
-      <c r="P19" s="111">
+      <c r="P19" s="91">
         <v>2.193548387096774</v>
       </c>
-      <c r="Q19" s="111">
+      <c r="Q19" s="91">
         <v>6.3592626728110595</v>
       </c>
-      <c r="R19" s="112">
+      <c r="R19" s="92">
         <v>8</v>
       </c>
-      <c r="S19" s="114">
+      <c r="S19" s="94">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A20" s="109" t="s">
+      <c r="A20" s="89" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="109" t="s">
+      <c r="B20" s="89" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="109" t="s">
+      <c r="C20" s="89" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="117">
+      <c r="D20" s="97">
         <v>309711744</v>
       </c>
-      <c r="E20" s="110">
+      <c r="E20" s="90">
         <v>7.96</v>
       </c>
-      <c r="F20" s="110">
+      <c r="F20" s="90">
         <v>6.5</v>
       </c>
-      <c r="G20" s="110">
+      <c r="G20" s="90">
         <v>7.1</v>
       </c>
-      <c r="H20" s="110">
+      <c r="H20" s="90">
         <v>7.61</v>
       </c>
-      <c r="I20" s="110">
+      <c r="I20" s="90">
         <v>3.9</v>
       </c>
-      <c r="J20" s="110">
+      <c r="J20" s="90">
         <v>9.83</v>
       </c>
-      <c r="K20" s="110">
+      <c r="K20" s="90">
         <v>9.5</v>
       </c>
-      <c r="L20" s="110">
+      <c r="L20" s="90">
         <v>8.33</v>
       </c>
-      <c r="M20" s="111">
+      <c r="M20" s="91">
         <v>4.617</v>
       </c>
-      <c r="N20" s="118">
+      <c r="N20" s="98">
         <v>14</v>
       </c>
-      <c r="O20" s="119">
+      <c r="O20" s="99">
         <v>0.45</v>
       </c>
-      <c r="P20" s="111">
+      <c r="P20" s="91">
         <v>1.5948387096774193</v>
       </c>
-      <c r="Q20" s="111">
+      <c r="Q20" s="91">
         <v>6.2118387096774192</v>
       </c>
-      <c r="R20" s="112">
+      <c r="R20" s="92">
         <v>8</v>
       </c>
-      <c r="S20" s="114">
+      <c r="S20" s="94">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A21" s="109" t="s">
+      <c r="A21" s="89" t="s">
         <v>104</v>
       </c>
-      <c r="B21" s="109" t="s">
+      <c r="B21" s="89" t="s">
         <v>105</v>
       </c>
-      <c r="C21" s="109" t="s">
+      <c r="C21" s="89" t="s">
         <v>106</v>
       </c>
-      <c r="D21" s="117">
+      <c r="D21" s="97">
         <v>406037596</v>
       </c>
-      <c r="E21" s="110"/>
-      <c r="F21" s="110"/>
-      <c r="G21" s="110"/>
-      <c r="H21" s="110"/>
-      <c r="I21" s="110"/>
-      <c r="J21" s="110"/>
-      <c r="K21" s="110"/>
-      <c r="L21" s="110"/>
-      <c r="M21" s="111"/>
-      <c r="N21" s="118">
-        <v>0</v>
-      </c>
-      <c r="O21" s="119">
-        <v>0</v>
-      </c>
-      <c r="P21" s="111">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="111" t="s">
+      <c r="E21" s="90"/>
+      <c r="F21" s="90"/>
+      <c r="G21" s="90"/>
+      <c r="H21" s="90"/>
+      <c r="I21" s="90"/>
+      <c r="J21" s="90"/>
+      <c r="K21" s="90"/>
+      <c r="L21" s="90"/>
+      <c r="M21" s="91"/>
+      <c r="N21" s="98">
+        <v>0</v>
+      </c>
+      <c r="O21" s="99">
+        <v>0</v>
+      </c>
+      <c r="P21" s="91">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R21" s="112" t="s">
+      <c r="R21" s="92" t="s">
         <v>271</v>
       </c>
-      <c r="S21" s="115"/>
+      <c r="S21" s="95"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A22" s="109" t="s">
+      <c r="A22" s="89" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="109" t="s">
+      <c r="B22" s="89" t="s">
         <v>109</v>
       </c>
-      <c r="C22" s="109" t="s">
+      <c r="C22" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="D22" s="117">
+      <c r="D22" s="97">
         <v>314612777</v>
       </c>
-      <c r="E22" s="110"/>
-      <c r="F22" s="110"/>
-      <c r="G22" s="110"/>
-      <c r="H22" s="110"/>
-      <c r="I22" s="110"/>
-      <c r="J22" s="110"/>
-      <c r="K22" s="110"/>
-      <c r="L22" s="110"/>
-      <c r="M22" s="111"/>
-      <c r="N22" s="118">
+      <c r="E22" s="90"/>
+      <c r="F22" s="90"/>
+      <c r="G22" s="90"/>
+      <c r="H22" s="90"/>
+      <c r="I22" s="90"/>
+      <c r="J22" s="90"/>
+      <c r="K22" s="90"/>
+      <c r="L22" s="90"/>
+      <c r="M22" s="91"/>
+      <c r="N22" s="98">
         <v>5</v>
       </c>
-      <c r="O22" s="119">
+      <c r="O22" s="99">
         <v>0.16</v>
       </c>
-      <c r="P22" s="111">
+      <c r="P22" s="91">
         <v>0.56774193548387097</v>
       </c>
-      <c r="Q22" s="111" t="s">
+      <c r="Q22" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R22" s="112">
+      <c r="R22" s="92">
         <v>5</v>
       </c>
-      <c r="S22" s="115"/>
+      <c r="S22" s="95"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A23" s="109" t="s">
+      <c r="A23" s="89" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="109" t="s">
+      <c r="B23" s="89" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="109" t="s">
+      <c r="C23" s="89" t="s">
         <v>114</v>
       </c>
-      <c r="D23" s="117">
+      <c r="D23" s="97">
         <v>414076695</v>
       </c>
-      <c r="E23" s="110"/>
-      <c r="F23" s="110"/>
-      <c r="G23" s="110"/>
-      <c r="H23" s="110"/>
-      <c r="I23" s="110"/>
-      <c r="J23" s="110"/>
-      <c r="K23" s="110"/>
-      <c r="L23" s="110"/>
-      <c r="M23" s="111"/>
-      <c r="N23" s="118">
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
+      <c r="G23" s="90"/>
+      <c r="H23" s="90"/>
+      <c r="I23" s="90"/>
+      <c r="J23" s="90"/>
+      <c r="K23" s="90"/>
+      <c r="L23" s="90"/>
+      <c r="M23" s="91"/>
+      <c r="N23" s="98">
         <v>2</v>
       </c>
-      <c r="O23" s="119">
+      <c r="O23" s="99">
         <v>0.06</v>
       </c>
-      <c r="P23" s="111">
+      <c r="P23" s="91">
         <v>0.25806451612903225</v>
       </c>
-      <c r="Q23" s="111" t="s">
+      <c r="Q23" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R23" s="112">
+      <c r="R23" s="92">
         <v>5</v>
       </c>
-      <c r="S23" s="115"/>
+      <c r="S23" s="95"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A24" s="109" t="s">
+      <c r="A24" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="109" t="s">
+      <c r="B24" s="89" t="s">
         <v>117</v>
       </c>
-      <c r="C24" s="109" t="s">
+      <c r="C24" s="89" t="s">
         <v>118</v>
       </c>
-      <c r="D24" s="117">
+      <c r="D24" s="97">
         <v>313353181</v>
       </c>
-      <c r="E24" s="110">
+      <c r="E24" s="90">
         <v>7.28</v>
       </c>
-      <c r="F24" s="110">
+      <c r="F24" s="90">
         <v>8.36</v>
       </c>
-      <c r="G24" s="110">
+      <c r="G24" s="90">
         <v>6.85</v>
       </c>
-      <c r="H24" s="110">
+      <c r="H24" s="90">
         <v>8.5500000000000007</v>
       </c>
-      <c r="I24" s="110">
+      <c r="I24" s="90">
         <v>3.2</v>
       </c>
-      <c r="J24" s="110">
+      <c r="J24" s="90">
         <v>6.25</v>
       </c>
-      <c r="K24" s="110">
+      <c r="K24" s="90">
         <v>3.95</v>
       </c>
-      <c r="L24" s="110">
+      <c r="L24" s="90">
         <v>7.91</v>
       </c>
-      <c r="M24" s="111">
+      <c r="M24" s="91">
         <v>4.0821428571428573</v>
       </c>
-      <c r="N24" s="118">
+      <c r="N24" s="98">
         <v>12</v>
       </c>
-      <c r="O24" s="119">
+      <c r="O24" s="99">
         <v>0.39</v>
       </c>
-      <c r="P24" s="111">
+      <c r="P24" s="91">
         <v>1.4064516129032258</v>
       </c>
-      <c r="Q24" s="111">
+      <c r="Q24" s="91">
         <v>5.4885944700460829</v>
       </c>
-      <c r="R24" s="112">
+      <c r="R24" s="92">
         <v>7</v>
       </c>
-      <c r="S24" s="114">
+      <c r="S24" s="94">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A25" s="109" t="s">
+      <c r="A25" s="89" t="s">
         <v>120</v>
       </c>
-      <c r="B25" s="109" t="s">
+      <c r="B25" s="89" t="s">
         <v>121</v>
       </c>
-      <c r="C25" s="109" t="s">
+      <c r="C25" s="89" t="s">
         <v>122</v>
       </c>
-      <c r="D25" s="117">
+      <c r="D25" s="97">
         <v>309275491</v>
       </c>
-      <c r="E25" s="110">
+      <c r="E25" s="90">
         <v>3.75</v>
       </c>
-      <c r="F25" s="110">
+      <c r="F25" s="90">
         <v>4</v>
       </c>
-      <c r="G25" s="110">
+      <c r="G25" s="90">
         <v>6.65</v>
       </c>
-      <c r="H25" s="110">
+      <c r="H25" s="90">
         <v>7.22</v>
       </c>
-      <c r="I25" s="110">
-        <v>0</v>
-      </c>
-      <c r="J25" s="110">
+      <c r="I25" s="90">
+        <v>0</v>
+      </c>
+      <c r="J25" s="90">
         <v>8.75</v>
       </c>
-      <c r="K25" s="110">
+      <c r="K25" s="90">
         <v>3.5</v>
       </c>
-      <c r="L25" s="110">
+      <c r="L25" s="90">
         <v>6.67</v>
       </c>
-      <c r="M25" s="111">
+      <c r="M25" s="91">
         <v>3.0998571428571426</v>
       </c>
-      <c r="N25" s="118">
+      <c r="N25" s="98">
         <v>15</v>
       </c>
-      <c r="O25" s="119">
+      <c r="O25" s="99">
         <v>0.48</v>
       </c>
-      <c r="P25" s="111">
+      <c r="P25" s="91">
         <v>1.7354838709677418</v>
       </c>
-      <c r="Q25" s="111">
+      <c r="Q25" s="91">
         <v>4.835341013824884</v>
       </c>
-      <c r="R25" s="112" t="s">
+      <c r="R25" s="92" t="s">
         <v>282</v>
       </c>
-      <c r="S25" s="114">
+      <c r="S25" s="94">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A26" s="109" t="s">
+      <c r="A26" s="89" t="s">
         <v>124</v>
       </c>
-      <c r="B26" s="109" t="s">
+      <c r="B26" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="109" t="s">
+      <c r="C26" s="89" t="s">
         <v>125</v>
       </c>
-      <c r="D26" s="117">
+      <c r="D26" s="97">
         <v>413035868</v>
       </c>
-      <c r="E26" s="110"/>
-      <c r="F26" s="110"/>
-      <c r="G26" s="110"/>
-      <c r="H26" s="110"/>
-      <c r="I26" s="110"/>
-      <c r="J26" s="110"/>
-      <c r="K26" s="110"/>
-      <c r="L26" s="110"/>
-      <c r="M26" s="111"/>
-      <c r="N26" s="118">
+      <c r="E26" s="90"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="90"/>
+      <c r="I26" s="90"/>
+      <c r="J26" s="90"/>
+      <c r="K26" s="90"/>
+      <c r="L26" s="90"/>
+      <c r="M26" s="91"/>
+      <c r="N26" s="98">
         <v>4</v>
       </c>
-      <c r="O26" s="119">
+      <c r="O26" s="99">
         <v>0.13</v>
       </c>
-      <c r="P26" s="111">
+      <c r="P26" s="91">
         <v>0.40387096774193543</v>
       </c>
-      <c r="Q26" s="111" t="s">
+      <c r="Q26" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R26" s="112">
+      <c r="R26" s="92">
         <v>5</v>
       </c>
-      <c r="S26" s="115"/>
+      <c r="S26" s="95"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A27" s="109" t="s">
+      <c r="A27" s="89" t="s">
         <v>127</v>
       </c>
-      <c r="B27" s="109" t="s">
+      <c r="B27" s="89" t="s">
         <v>128</v>
       </c>
-      <c r="C27" s="109" t="s">
+      <c r="C27" s="89" t="s">
         <v>129</v>
       </c>
-      <c r="D27" s="117">
+      <c r="D27" s="97">
         <v>310284631</v>
       </c>
-      <c r="E27" s="110"/>
-      <c r="F27" s="110"/>
-      <c r="G27" s="110"/>
-      <c r="H27" s="110"/>
-      <c r="I27" s="110"/>
-      <c r="J27" s="110"/>
-      <c r="K27" s="110"/>
-      <c r="L27" s="110"/>
-      <c r="M27" s="111"/>
-      <c r="N27" s="118">
+      <c r="E27" s="90"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="90"/>
+      <c r="J27" s="90"/>
+      <c r="K27" s="90"/>
+      <c r="L27" s="90"/>
+      <c r="M27" s="91"/>
+      <c r="N27" s="98">
         <v>2</v>
       </c>
-      <c r="O27" s="119">
+      <c r="O27" s="99">
         <v>0.06</v>
       </c>
-      <c r="P27" s="111">
+      <c r="P27" s="91">
         <v>0.23225806451612907</v>
       </c>
-      <c r="Q27" s="111" t="s">
+      <c r="Q27" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R27" s="112">
+      <c r="R27" s="92">
         <v>5</v>
       </c>
-      <c r="S27" s="115"/>
+      <c r="S27" s="95"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A28" s="109" t="s">
+      <c r="A28" s="89" t="s">
         <v>128</v>
       </c>
-      <c r="B28" s="109" t="s">
+      <c r="B28" s="89" t="s">
         <v>131</v>
       </c>
-      <c r="C28" s="109" t="s">
+      <c r="C28" s="89" t="s">
         <v>132</v>
       </c>
-      <c r="D28" s="117">
+      <c r="D28" s="97">
         <v>310294548</v>
       </c>
-      <c r="E28" s="110">
+      <c r="E28" s="90">
         <v>5.6</v>
       </c>
-      <c r="F28" s="110">
+      <c r="F28" s="90">
         <v>3.27</v>
       </c>
-      <c r="G28" s="110">
+      <c r="G28" s="90">
         <v>7</v>
       </c>
-      <c r="H28" s="110">
+      <c r="H28" s="90">
         <v>4.38</v>
       </c>
-      <c r="I28" s="110">
-        <v>0</v>
-      </c>
-      <c r="J28" s="110">
+      <c r="I28" s="90">
+        <v>0</v>
+      </c>
+      <c r="J28" s="90">
         <v>5</v>
       </c>
-      <c r="K28" s="110">
+      <c r="K28" s="90">
         <v>5</v>
       </c>
-      <c r="L28" s="110">
+      <c r="L28" s="90">
         <v>5.41</v>
       </c>
-      <c r="M28" s="111">
+      <c r="M28" s="91">
         <v>2.8422857142857141</v>
       </c>
-      <c r="N28" s="118">
+      <c r="N28" s="98">
         <v>7</v>
       </c>
-      <c r="O28" s="119">
+      <c r="O28" s="99">
         <v>0.23</v>
       </c>
-      <c r="P28" s="111">
+      <c r="P28" s="91">
         <v>0.78064516129032258</v>
       </c>
-      <c r="Q28" s="111">
+      <c r="Q28" s="91">
         <v>4.8</v>
       </c>
-      <c r="R28" s="112" t="s">
+      <c r="R28" s="92" t="s">
         <v>282</v>
       </c>
-      <c r="S28" s="114">
+      <c r="S28" s="94">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A29" s="109" t="s">
+      <c r="A29" s="89" t="s">
         <v>134</v>
       </c>
-      <c r="B29" s="109" t="s">
+      <c r="B29" s="89" t="s">
         <v>135</v>
       </c>
-      <c r="C29" s="109" t="s">
+      <c r="C29" s="89" t="s">
         <v>136</v>
       </c>
-      <c r="D29" s="117">
+      <c r="D29" s="97">
         <v>309169523</v>
       </c>
-      <c r="E29" s="110"/>
-      <c r="F29" s="110"/>
-      <c r="G29" s="110"/>
-      <c r="H29" s="110"/>
-      <c r="I29" s="110"/>
-      <c r="J29" s="110"/>
-      <c r="K29" s="110"/>
-      <c r="L29" s="110"/>
-      <c r="M29" s="111"/>
-      <c r="N29" s="118">
+      <c r="E29" s="90"/>
+      <c r="F29" s="90"/>
+      <c r="G29" s="90"/>
+      <c r="H29" s="90"/>
+      <c r="I29" s="90"/>
+      <c r="J29" s="90"/>
+      <c r="K29" s="90"/>
+      <c r="L29" s="90"/>
+      <c r="M29" s="91"/>
+      <c r="N29" s="98">
         <v>3</v>
       </c>
-      <c r="O29" s="119">
+      <c r="O29" s="99">
         <v>0.1</v>
       </c>
-      <c r="P29" s="111">
+      <c r="P29" s="91">
         <v>0.21935483870967742</v>
       </c>
-      <c r="Q29" s="111" t="s">
+      <c r="Q29" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R29" s="112">
+      <c r="R29" s="92">
         <v>5</v>
       </c>
-      <c r="S29" s="115"/>
+      <c r="S29" s="95"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A30" s="109" t="s">
+      <c r="A30" s="89" t="s">
         <v>138</v>
       </c>
-      <c r="B30" s="109" t="s">
+      <c r="B30" s="89" t="s">
         <v>139</v>
       </c>
-      <c r="C30" s="109" t="s">
+      <c r="C30" s="89" t="s">
         <v>140</v>
       </c>
-      <c r="D30" s="117">
+      <c r="D30" s="97">
         <v>415005614</v>
       </c>
-      <c r="E30" s="110"/>
-      <c r="F30" s="110"/>
-      <c r="G30" s="110"/>
-      <c r="H30" s="110"/>
-      <c r="I30" s="110"/>
-      <c r="J30" s="110"/>
-      <c r="K30" s="110"/>
-      <c r="L30" s="110"/>
-      <c r="M30" s="111"/>
-      <c r="N30" s="118">
-        <v>0</v>
-      </c>
-      <c r="O30" s="119">
-        <v>0</v>
-      </c>
-      <c r="P30" s="111">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="111" t="s">
+      <c r="E30" s="90"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="90"/>
+      <c r="I30" s="90"/>
+      <c r="J30" s="90"/>
+      <c r="K30" s="90"/>
+      <c r="L30" s="90"/>
+      <c r="M30" s="91"/>
+      <c r="N30" s="98">
+        <v>0</v>
+      </c>
+      <c r="O30" s="99">
+        <v>0</v>
+      </c>
+      <c r="P30" s="91">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R30" s="112" t="s">
+      <c r="R30" s="92" t="s">
         <v>271</v>
       </c>
-      <c r="S30" s="115"/>
+      <c r="S30" s="95"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A31" s="109" t="s">
+      <c r="A31" s="89" t="s">
         <v>142</v>
       </c>
-      <c r="B31" s="109" t="s">
+      <c r="B31" s="89" t="s">
         <v>143</v>
       </c>
-      <c r="C31" s="109" t="s">
+      <c r="C31" s="89" t="s">
         <v>144</v>
       </c>
-      <c r="D31" s="117">
+      <c r="D31" s="97">
         <v>314280790</v>
       </c>
-      <c r="E31" s="110">
+      <c r="E31" s="90">
         <v>7.15</v>
       </c>
-      <c r="F31" s="110">
+      <c r="F31" s="90">
         <v>6.35</v>
       </c>
-      <c r="G31" s="110">
+      <c r="G31" s="90">
         <v>9.6</v>
       </c>
-      <c r="H31" s="110">
+      <c r="H31" s="90">
         <v>9.33</v>
       </c>
-      <c r="I31" s="110">
+      <c r="I31" s="90">
         <v>10</v>
       </c>
-      <c r="J31" s="110">
+      <c r="J31" s="90">
         <v>10</v>
       </c>
-      <c r="K31" s="110">
+      <c r="K31" s="90">
         <v>9.5</v>
       </c>
-      <c r="L31" s="110">
+      <c r="L31" s="90">
         <v>8.33</v>
       </c>
-      <c r="M31" s="111">
+      <c r="M31" s="91">
         <v>5.1651428571428566</v>
       </c>
-      <c r="N31" s="118">
+      <c r="N31" s="98">
         <v>25</v>
       </c>
-      <c r="O31" s="119">
+      <c r="O31" s="99">
         <v>0.81</v>
       </c>
-      <c r="P31" s="111">
+      <c r="P31" s="91">
         <v>3.0916129032258066</v>
       </c>
-      <c r="Q31" s="111">
+      <c r="Q31" s="91">
         <v>8.2567557603686623</v>
       </c>
-      <c r="R31" s="112">
+      <c r="R31" s="92">
         <v>9.9567557603686616</v>
       </c>
-      <c r="S31" s="114">
+      <c r="S31" s="94">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A32" s="109" t="s">
+      <c r="A32" s="89" t="s">
         <v>146</v>
       </c>
-      <c r="B32" s="109" t="s">
+      <c r="B32" s="89" t="s">
         <v>147</v>
       </c>
-      <c r="C32" s="109" t="s">
+      <c r="C32" s="89" t="s">
         <v>102</v>
       </c>
-      <c r="D32" s="117">
+      <c r="D32" s="97">
         <v>312107534</v>
       </c>
-      <c r="E32" s="110">
+      <c r="E32" s="90">
         <v>0.5</v>
       </c>
-      <c r="F32" s="110">
+      <c r="F32" s="90">
         <v>1.5</v>
       </c>
-      <c r="G32" s="110"/>
-      <c r="H32" s="110"/>
-      <c r="I32" s="110"/>
-      <c r="J32" s="110"/>
-      <c r="K32" s="110"/>
-      <c r="L32" s="110"/>
-      <c r="M32" s="111"/>
-      <c r="N32" s="118">
+      <c r="G32" s="90"/>
+      <c r="H32" s="90"/>
+      <c r="I32" s="90"/>
+      <c r="J32" s="90"/>
+      <c r="K32" s="90"/>
+      <c r="L32" s="90"/>
+      <c r="M32" s="91"/>
+      <c r="N32" s="98">
         <v>2</v>
       </c>
-      <c r="O32" s="119">
+      <c r="O32" s="99">
         <v>0.06</v>
       </c>
-      <c r="P32" s="111">
+      <c r="P32" s="91">
         <v>0.21935483870967742</v>
       </c>
-      <c r="Q32" s="111">
+      <c r="Q32" s="91">
         <v>5</v>
       </c>
-      <c r="R32" s="112">
+      <c r="R32" s="92">
         <v>5</v>
       </c>
-      <c r="S32" s="115"/>
+      <c r="S32" s="95"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A33" s="109" t="s">
+      <c r="A33" s="89" t="s">
         <v>146</v>
       </c>
-      <c r="B33" s="109" t="s">
+      <c r="B33" s="89" t="s">
         <v>149</v>
       </c>
-      <c r="C33" s="109" t="s">
+      <c r="C33" s="89" t="s">
         <v>150</v>
       </c>
-      <c r="D33" s="117">
+      <c r="D33" s="97">
         <v>412010675</v>
       </c>
-      <c r="E33" s="110"/>
-      <c r="F33" s="110"/>
-      <c r="G33" s="110"/>
-      <c r="H33" s="110"/>
-      <c r="I33" s="110"/>
-      <c r="J33" s="110"/>
-      <c r="K33" s="110"/>
-      <c r="L33" s="110"/>
-      <c r="M33" s="111"/>
-      <c r="N33" s="118">
-        <v>0</v>
-      </c>
-      <c r="O33" s="119">
-        <v>0</v>
-      </c>
-      <c r="P33" s="111">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="111" t="s">
+      <c r="E33" s="90"/>
+      <c r="F33" s="90"/>
+      <c r="G33" s="90"/>
+      <c r="H33" s="90"/>
+      <c r="I33" s="90"/>
+      <c r="J33" s="90"/>
+      <c r="K33" s="90"/>
+      <c r="L33" s="90"/>
+      <c r="M33" s="91"/>
+      <c r="N33" s="98">
+        <v>0</v>
+      </c>
+      <c r="O33" s="99">
+        <v>0</v>
+      </c>
+      <c r="P33" s="91">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R33" s="112" t="s">
+      <c r="R33" s="92" t="s">
         <v>271</v>
       </c>
-      <c r="S33" s="115"/>
+      <c r="S33" s="95"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A34" s="109" t="s">
+      <c r="A34" s="89" t="s">
         <v>152</v>
       </c>
-      <c r="B34" s="109" t="s">
+      <c r="B34" s="89" t="s">
         <v>153</v>
       </c>
-      <c r="C34" s="109" t="s">
+      <c r="C34" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="117">
+      <c r="D34" s="97">
         <v>310261658</v>
       </c>
-      <c r="E34" s="110">
+      <c r="E34" s="90">
         <v>8.8000000000000007</v>
       </c>
-      <c r="F34" s="110">
+      <c r="F34" s="90">
         <v>9.18</v>
       </c>
-      <c r="G34" s="110">
+      <c r="G34" s="90">
         <v>7.55</v>
       </c>
-      <c r="H34" s="110">
+      <c r="H34" s="90">
         <v>7.88</v>
       </c>
-      <c r="I34" s="110"/>
-      <c r="J34" s="110"/>
-      <c r="K34" s="110"/>
-      <c r="L34" s="110"/>
-      <c r="M34" s="111"/>
-      <c r="N34" s="118">
+      <c r="I34" s="90"/>
+      <c r="J34" s="90"/>
+      <c r="K34" s="90"/>
+      <c r="L34" s="90"/>
+      <c r="M34" s="91"/>
+      <c r="N34" s="98">
         <v>17</v>
       </c>
-      <c r="O34" s="119">
+      <c r="O34" s="99">
         <v>0.55000000000000004</v>
       </c>
-      <c r="P34" s="111">
+      <c r="P34" s="91">
         <v>1.8658064516129036</v>
       </c>
-      <c r="Q34" s="111">
+      <c r="Q34" s="91">
         <v>5</v>
       </c>
-      <c r="R34" s="112">
+      <c r="R34" s="92">
         <v>5</v>
       </c>
-      <c r="S34" s="115"/>
+      <c r="S34" s="95"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A35" s="109" t="s">
+      <c r="A35" s="89" t="s">
         <v>155</v>
       </c>
-      <c r="B35" s="109" t="s">
+      <c r="B35" s="89" t="s">
         <v>156</v>
       </c>
-      <c r="C35" s="109" t="s">
+      <c r="C35" s="89" t="s">
         <v>157</v>
       </c>
-      <c r="D35" s="117">
+      <c r="D35" s="97">
         <v>311176968</v>
       </c>
-      <c r="E35" s="110">
+      <c r="E35" s="90">
         <v>0.91</v>
       </c>
-      <c r="F35" s="110">
+      <c r="F35" s="90">
         <v>2</v>
       </c>
-      <c r="G35" s="110"/>
-      <c r="H35" s="110"/>
-      <c r="I35" s="110"/>
-      <c r="J35" s="110"/>
-      <c r="K35" s="110" t="s">
+      <c r="G35" s="90"/>
+      <c r="H35" s="90"/>
+      <c r="I35" s="90"/>
+      <c r="J35" s="90"/>
+      <c r="K35" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="L35" s="110"/>
-      <c r="M35" s="111"/>
-      <c r="N35" s="118">
+      <c r="L35" s="90"/>
+      <c r="M35" s="91"/>
+      <c r="N35" s="98">
         <v>2</v>
       </c>
-      <c r="O35" s="119">
+      <c r="O35" s="99">
         <v>0.06</v>
       </c>
-      <c r="P35" s="111">
+      <c r="P35" s="91">
         <v>0.20645161290322581</v>
       </c>
-      <c r="Q35" s="111">
+      <c r="Q35" s="91">
         <v>5</v>
       </c>
-      <c r="R35" s="112">
+      <c r="R35" s="92">
         <v>5</v>
       </c>
-      <c r="S35" s="115"/>
+      <c r="S35" s="95"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A36" s="109" t="s">
+      <c r="A36" s="89" t="s">
         <v>159</v>
       </c>
-      <c r="B36" s="109" t="s">
+      <c r="B36" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="C36" s="109" t="s">
+      <c r="C36" s="89" t="s">
         <v>160</v>
       </c>
-      <c r="D36" s="117">
+      <c r="D36" s="97">
         <v>309137575</v>
       </c>
-      <c r="E36" s="110">
+      <c r="E36" s="90">
         <v>4.4000000000000004</v>
       </c>
-      <c r="F36" s="110">
+      <c r="F36" s="90">
         <v>5.2</v>
       </c>
-      <c r="G36" s="110">
+      <c r="G36" s="90">
         <v>7.6</v>
       </c>
-      <c r="H36" s="110">
+      <c r="H36" s="90">
         <v>7.55</v>
       </c>
-      <c r="I36" s="110">
+      <c r="I36" s="90">
         <v>2</v>
       </c>
-      <c r="J36" s="110">
+      <c r="J36" s="90">
         <v>6.75</v>
       </c>
-      <c r="K36" s="110"/>
-      <c r="L36" s="110"/>
-      <c r="M36" s="111">
+      <c r="K36" s="90"/>
+      <c r="L36" s="90"/>
+      <c r="M36" s="91">
         <v>2.4964285714285719</v>
       </c>
-      <c r="N36" s="118">
+      <c r="N36" s="98">
         <v>14</v>
       </c>
-      <c r="O36" s="119">
+      <c r="O36" s="99">
         <v>0.45</v>
       </c>
-      <c r="P36" s="111">
+      <c r="P36" s="91">
         <v>1.5393548387096774</v>
       </c>
-      <c r="Q36" s="111">
+      <c r="Q36" s="91">
         <v>4.035783410138249</v>
       </c>
-      <c r="R36" s="112">
+      <c r="R36" s="92">
         <v>5</v>
       </c>
-      <c r="S36" s="115"/>
+      <c r="S36" s="95"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A37" s="109" t="s">
+      <c r="A37" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="109" t="s">
+      <c r="B37" s="89" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="109" t="s">
+      <c r="C37" s="89" t="s">
         <v>162</v>
       </c>
-      <c r="D37" s="117">
+      <c r="D37" s="97">
         <v>314184935</v>
       </c>
-      <c r="E37" s="110">
+      <c r="E37" s="90">
         <v>7.9</v>
       </c>
-      <c r="F37" s="110">
+      <c r="F37" s="90">
         <v>6.32</v>
       </c>
-      <c r="G37" s="110">
+      <c r="G37" s="90">
         <v>8</v>
       </c>
-      <c r="H37" s="110">
+      <c r="H37" s="90">
         <v>6.38</v>
       </c>
-      <c r="I37" s="110">
+      <c r="I37" s="90">
         <v>1.6</v>
       </c>
-      <c r="J37" s="110">
+      <c r="J37" s="90">
         <v>5.5</v>
       </c>
-      <c r="K37" s="110">
+      <c r="K37" s="90">
         <v>8</v>
       </c>
-      <c r="L37" s="110">
+      <c r="L37" s="90">
         <v>10</v>
       </c>
-      <c r="M37" s="111">
+      <c r="M37" s="91">
         <v>4.298571428571428</v>
       </c>
-      <c r="N37" s="118">
+      <c r="N37" s="98">
         <v>21</v>
       </c>
-      <c r="O37" s="119">
+      <c r="O37" s="99">
         <v>0.68</v>
       </c>
-      <c r="P37" s="111">
+      <c r="P37" s="91">
         <v>2.3780645161290326</v>
       </c>
-      <c r="Q37" s="111">
+      <c r="Q37" s="91">
         <v>6.6766359447004611</v>
       </c>
-      <c r="R37" s="112">
+      <c r="R37" s="92">
         <v>9</v>
       </c>
-      <c r="S37" s="114">
+      <c r="S37" s="94">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A38" s="109" t="s">
+      <c r="A38" s="89" t="s">
         <v>164</v>
       </c>
-      <c r="B38" s="109" t="s">
+      <c r="B38" s="89" t="s">
         <v>165</v>
       </c>
-      <c r="C38" s="109" t="s">
+      <c r="C38" s="89" t="s">
         <v>166</v>
       </c>
-      <c r="D38" s="117">
+      <c r="D38" s="97">
         <v>314244624</v>
       </c>
-      <c r="E38" s="110">
+      <c r="E38" s="90">
         <v>2</v>
       </c>
-      <c r="F38" s="110">
+      <c r="F38" s="90">
         <v>1.64</v>
       </c>
-      <c r="G38" s="110">
+      <c r="G38" s="90">
         <v>4.8</v>
       </c>
-      <c r="H38" s="110">
+      <c r="H38" s="90">
         <v>7.5</v>
       </c>
-      <c r="I38" s="110">
+      <c r="I38" s="90">
         <v>3.5</v>
       </c>
-      <c r="J38" s="110">
+      <c r="J38" s="90">
         <v>2.16</v>
       </c>
-      <c r="K38" s="110">
+      <c r="K38" s="90">
         <v>2.25</v>
       </c>
-      <c r="L38" s="110">
+      <c r="L38" s="90">
         <v>3.33</v>
       </c>
-      <c r="M38" s="111">
+      <c r="M38" s="91">
         <v>2.0871428571428572</v>
       </c>
-      <c r="N38" s="118">
+      <c r="N38" s="98">
         <v>21</v>
       </c>
-      <c r="O38" s="119">
+      <c r="O38" s="99">
         <v>0.68</v>
       </c>
-      <c r="P38" s="111">
+      <c r="P38" s="91">
         <v>2.4774193548387098</v>
       </c>
-      <c r="Q38" s="111">
+      <c r="Q38" s="91">
         <v>4.564562211981567</v>
       </c>
-      <c r="R38" s="112" t="s">
+      <c r="R38" s="92" t="s">
         <v>282</v>
       </c>
-      <c r="S38" s="114">
+      <c r="S38" s="94">
         <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A39" s="109" t="s">
+      <c r="A39" s="89" t="s">
         <v>168</v>
       </c>
-      <c r="B39" s="109" t="s">
+      <c r="B39" s="89" t="s">
         <v>169</v>
       </c>
-      <c r="C39" s="109" t="s">
+      <c r="C39" s="89" t="s">
         <v>170</v>
       </c>
-      <c r="D39" s="117">
+      <c r="D39" s="97">
         <v>313308679</v>
       </c>
-      <c r="E39" s="110"/>
-      <c r="F39" s="110"/>
-      <c r="G39" s="110"/>
-      <c r="H39" s="110"/>
-      <c r="I39" s="110"/>
-      <c r="J39" s="110"/>
-      <c r="K39" s="110"/>
-      <c r="L39" s="110"/>
-      <c r="M39" s="111"/>
-      <c r="N39" s="118">
+      <c r="E39" s="90"/>
+      <c r="F39" s="90"/>
+      <c r="G39" s="90"/>
+      <c r="H39" s="90"/>
+      <c r="I39" s="90"/>
+      <c r="J39" s="90"/>
+      <c r="K39" s="90"/>
+      <c r="L39" s="90"/>
+      <c r="M39" s="91"/>
+      <c r="N39" s="98">
         <v>3</v>
       </c>
-      <c r="O39" s="119">
+      <c r="O39" s="99">
         <v>0.1</v>
       </c>
-      <c r="P39" s="111">
+      <c r="P39" s="91">
         <v>0.34838709677419355</v>
       </c>
-      <c r="Q39" s="111" t="s">
+      <c r="Q39" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R39" s="112">
+      <c r="R39" s="92">
         <v>5</v>
       </c>
-      <c r="S39" s="115"/>
+      <c r="S39" s="95"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A40" s="109" t="s">
+      <c r="A40" s="89" t="s">
         <v>172</v>
       </c>
-      <c r="B40" s="109" t="s">
+      <c r="B40" s="89" t="s">
         <v>173</v>
       </c>
-      <c r="C40" s="109" t="s">
+      <c r="C40" s="89" t="s">
         <v>174</v>
       </c>
-      <c r="D40" s="117">
+      <c r="D40" s="97">
         <v>313073014</v>
       </c>
-      <c r="E40" s="110"/>
-      <c r="F40" s="110"/>
-      <c r="G40" s="110"/>
-      <c r="H40" s="110">
+      <c r="E40" s="90"/>
+      <c r="F40" s="90"/>
+      <c r="G40" s="90"/>
+      <c r="H40" s="90">
         <v>7.11</v>
       </c>
-      <c r="I40" s="110"/>
-      <c r="J40" s="110"/>
-      <c r="K40" s="110"/>
-      <c r="L40" s="110"/>
-      <c r="M40" s="111"/>
-      <c r="N40" s="118">
+      <c r="I40" s="90"/>
+      <c r="J40" s="90"/>
+      <c r="K40" s="90"/>
+      <c r="L40" s="90"/>
+      <c r="M40" s="91"/>
+      <c r="N40" s="98">
         <v>8</v>
       </c>
-      <c r="O40" s="119">
+      <c r="O40" s="99">
         <v>0.26</v>
       </c>
-      <c r="P40" s="111">
+      <c r="P40" s="91">
         <v>0.85161290322580641</v>
       </c>
-      <c r="Q40" s="111">
+      <c r="Q40" s="91">
         <v>5</v>
       </c>
-      <c r="R40" s="112">
+      <c r="R40" s="92">
         <v>5</v>
       </c>
-      <c r="S40" s="115"/>
+      <c r="S40" s="95"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A41" s="109" t="s">
+      <c r="A41" s="89" t="s">
         <v>176</v>
       </c>
-      <c r="B41" s="109" t="s">
+      <c r="B41" s="89" t="s">
         <v>177</v>
       </c>
-      <c r="C41" s="109" t="s">
+      <c r="C41" s="89" t="s">
         <v>178</v>
       </c>
-      <c r="D41" s="117">
+      <c r="D41" s="97">
         <v>312236942</v>
       </c>
-      <c r="E41" s="110">
+      <c r="E41" s="90">
         <v>4.68</v>
       </c>
-      <c r="F41" s="110">
+      <c r="F41" s="90">
         <v>3</v>
       </c>
-      <c r="G41" s="110"/>
-      <c r="H41" s="110"/>
-      <c r="I41" s="110"/>
-      <c r="J41" s="110"/>
-      <c r="K41" s="110"/>
-      <c r="L41" s="110"/>
-      <c r="M41" s="111"/>
-      <c r="N41" s="118">
+      <c r="G41" s="90"/>
+      <c r="H41" s="90"/>
+      <c r="I41" s="90"/>
+      <c r="J41" s="90"/>
+      <c r="K41" s="90"/>
+      <c r="L41" s="90"/>
+      <c r="M41" s="91"/>
+      <c r="N41" s="98">
         <v>7</v>
       </c>
-      <c r="O41" s="119">
+      <c r="O41" s="99">
         <v>0.23</v>
       </c>
-      <c r="P41" s="111">
+      <c r="P41" s="91">
         <v>0.71612903225806457</v>
       </c>
-      <c r="Q41" s="111">
+      <c r="Q41" s="91">
         <v>5</v>
       </c>
-      <c r="R41" s="112">
+      <c r="R41" s="92">
         <v>5</v>
       </c>
-      <c r="S41" s="115"/>
+      <c r="S41" s="95"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A42" s="109" t="s">
+      <c r="A42" s="89" t="s">
         <v>180</v>
       </c>
-      <c r="B42" s="109" t="s">
+      <c r="B42" s="89" t="s">
         <v>181</v>
       </c>
-      <c r="C42" s="109" t="s">
+      <c r="C42" s="89" t="s">
         <v>182</v>
       </c>
-      <c r="D42" s="117">
+      <c r="D42" s="97">
         <v>307154419</v>
       </c>
-      <c r="E42" s="110"/>
-      <c r="F42" s="110"/>
-      <c r="G42" s="110"/>
-      <c r="H42" s="110"/>
-      <c r="I42" s="110"/>
-      <c r="J42" s="110"/>
-      <c r="K42" s="110"/>
-      <c r="L42" s="110"/>
-      <c r="M42" s="111"/>
-      <c r="N42" s="118">
-        <v>0</v>
-      </c>
-      <c r="O42" s="119">
-        <v>0</v>
-      </c>
-      <c r="P42" s="111">
-        <v>0</v>
-      </c>
-      <c r="Q42" s="111" t="s">
+      <c r="E42" s="90"/>
+      <c r="F42" s="90"/>
+      <c r="G42" s="90"/>
+      <c r="H42" s="90"/>
+      <c r="I42" s="90"/>
+      <c r="J42" s="90"/>
+      <c r="K42" s="90"/>
+      <c r="L42" s="90"/>
+      <c r="M42" s="91"/>
+      <c r="N42" s="98">
+        <v>0</v>
+      </c>
+      <c r="O42" s="99">
+        <v>0</v>
+      </c>
+      <c r="P42" s="91">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R42" s="112" t="s">
+      <c r="R42" s="92" t="s">
         <v>271</v>
       </c>
-      <c r="S42" s="115"/>
+      <c r="S42" s="95"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A43" s="109" t="s">
+      <c r="A43" s="89" t="s">
         <v>180</v>
       </c>
-      <c r="B43" s="109" t="s">
+      <c r="B43" s="89" t="s">
         <v>152</v>
       </c>
-      <c r="C43" s="109" t="s">
+      <c r="C43" s="89" t="s">
         <v>184</v>
       </c>
-      <c r="D43" s="117">
+      <c r="D43" s="97">
         <v>314254177</v>
       </c>
-      <c r="E43" s="110">
-        <v>0</v>
-      </c>
-      <c r="F43" s="110">
-        <v>0</v>
-      </c>
-      <c r="G43" s="110">
+      <c r="E43" s="90">
+        <v>0</v>
+      </c>
+      <c r="F43" s="90">
+        <v>0</v>
+      </c>
+      <c r="G43" s="90">
         <v>4.7</v>
       </c>
-      <c r="H43" s="110">
+      <c r="H43" s="90">
         <v>6.22</v>
       </c>
-      <c r="I43" s="110">
-        <v>0</v>
-      </c>
-      <c r="J43" s="110">
+      <c r="I43" s="90">
+        <v>0</v>
+      </c>
+      <c r="J43" s="90">
         <v>3.17</v>
       </c>
-      <c r="K43" s="110">
+      <c r="K43" s="90">
         <v>0.2</v>
       </c>
-      <c r="L43" s="110">
-        <v>0</v>
-      </c>
-      <c r="M43" s="111">
+      <c r="L43" s="90">
+        <v>0</v>
+      </c>
+      <c r="M43" s="91">
         <v>1.0889999999999997</v>
       </c>
-      <c r="N43" s="118">
+      <c r="N43" s="98">
         <v>11</v>
       </c>
-      <c r="O43" s="119">
+      <c r="O43" s="99">
         <v>0.35</v>
       </c>
-      <c r="P43" s="111">
+      <c r="P43" s="91">
         <v>1.2683870967741937</v>
       </c>
-      <c r="Q43" s="111">
+      <c r="Q43" s="91">
         <v>2.3573870967741932</v>
       </c>
-      <c r="R43" s="112" t="s">
+      <c r="R43" s="92" t="s">
         <v>282</v>
       </c>
-      <c r="S43" s="114">
+      <c r="S43" s="94">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización 19 de junio de 2019
Se incluye el examen extraordinario de MAF, las calificaciones finales del curso 2019-2 y se comienzan las notas de cálculo tensorial para apoyo del Tema 1 La física y la geometría.
</commit_message>
<xml_diff>
--- a/MAF-2019-2-Calificaciones.xlsx
+++ b/MAF-2019-2-Calificaciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavo/Documents/Matematicas Avanzadas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3672243-69C0-DA4D-8791-66680BB54453}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11761270-F148-AD48-BAA9-460DF663629A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="1960" windowWidth="14440" windowHeight="13840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Listado de Inscripción " sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="287">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -891,6 +891,9 @@
   </si>
   <si>
     <t>Porce_Ejercicios</t>
+  </si>
+  <si>
+    <t>Acta</t>
   </si>
 </sst>
 </file>
@@ -1584,34 +1587,34 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2026,7 +2029,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B52"/>
+      <selection activeCell="J11" sqref="J11:J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5466,7 +5469,7 @@
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="6"/>
-      <c r="K1" s="109" t="s">
+      <c r="K1" s="112" t="s">
         <v>11</v>
       </c>
       <c r="L1" s="101"/>
@@ -5692,9 +5695,9 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="107"/>
-      <c r="G4" s="108"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="110"/>
+      <c r="G4" s="111"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="4"/>
@@ -5745,35 +5748,35 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="110" t="s">
+      <c r="E5" s="106" t="s">
         <v>190</v>
       </c>
-      <c r="F5" s="111"/>
-      <c r="G5" s="112"/>
-      <c r="H5" s="110" t="s">
+      <c r="F5" s="107"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="106" t="s">
         <v>191</v>
       </c>
-      <c r="I5" s="112"/>
-      <c r="J5" s="110" t="s">
+      <c r="I5" s="108"/>
+      <c r="J5" s="106" t="s">
         <v>192</v>
       </c>
-      <c r="K5" s="111"/>
-      <c r="L5" s="111"/>
-      <c r="M5" s="112"/>
-      <c r="N5" s="110" t="s">
+      <c r="K5" s="107"/>
+      <c r="L5" s="107"/>
+      <c r="M5" s="108"/>
+      <c r="N5" s="106" t="s">
         <v>193</v>
       </c>
-      <c r="O5" s="111"/>
-      <c r="P5" s="112"/>
-      <c r="Q5" s="110" t="s">
+      <c r="O5" s="107"/>
+      <c r="P5" s="108"/>
+      <c r="Q5" s="106" t="s">
         <v>194</v>
       </c>
-      <c r="R5" s="111"/>
-      <c r="S5" s="111"/>
-      <c r="T5" s="111"/>
-      <c r="U5" s="111"/>
-      <c r="V5" s="111"/>
-      <c r="W5" s="112"/>
+      <c r="R5" s="107"/>
+      <c r="S5" s="107"/>
+      <c r="T5" s="107"/>
+      <c r="U5" s="107"/>
+      <c r="V5" s="107"/>
+      <c r="W5" s="108"/>
       <c r="X5" s="105" t="s">
         <v>195</v>
       </c>
@@ -14706,12 +14709,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="N5:P5"/>
-    <mergeCell ref="X5:AA5"/>
-    <mergeCell ref="Q5:W5"/>
-    <mergeCell ref="AG5:AI5"/>
-    <mergeCell ref="AB5:AD5"/>
-    <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="E4:G4"/>
@@ -14719,6 +14716,12 @@
     <mergeCell ref="J5:M5"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="H5:I5"/>
+    <mergeCell ref="N5:P5"/>
+    <mergeCell ref="X5:AA5"/>
+    <mergeCell ref="Q5:W5"/>
+    <mergeCell ref="AG5:AI5"/>
+    <mergeCell ref="AB5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -16581,42 +16584,42 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="114" t="s">
+      <c r="E6" s="118" t="s">
         <v>205</v>
       </c>
-      <c r="F6" s="115"/>
-      <c r="G6" s="114" t="s">
+      <c r="F6" s="114"/>
+      <c r="G6" s="118" t="s">
         <v>213</v>
       </c>
-      <c r="H6" s="115"/>
-      <c r="I6" s="114" t="s">
+      <c r="H6" s="114"/>
+      <c r="I6" s="118" t="s">
         <v>224</v>
       </c>
-      <c r="J6" s="115"/>
-      <c r="K6" s="116" t="s">
+      <c r="J6" s="114"/>
+      <c r="K6" s="115" t="s">
         <v>229</v>
       </c>
-      <c r="L6" s="115"/>
-      <c r="M6" s="116" t="s">
+      <c r="L6" s="114"/>
+      <c r="M6" s="115" t="s">
         <v>234</v>
       </c>
-      <c r="N6" s="115"/>
-      <c r="O6" s="116" t="s">
+      <c r="N6" s="114"/>
+      <c r="O6" s="115" t="s">
         <v>235</v>
       </c>
-      <c r="P6" s="115"/>
-      <c r="Q6" s="116" t="s">
+      <c r="P6" s="114"/>
+      <c r="Q6" s="115" t="s">
         <v>236</v>
       </c>
-      <c r="R6" s="115"/>
-      <c r="S6" s="116" t="s">
+      <c r="R6" s="114"/>
+      <c r="S6" s="115" t="s">
         <v>237</v>
       </c>
-      <c r="T6" s="115"/>
-      <c r="U6" s="113" t="s">
+      <c r="T6" s="114"/>
+      <c r="U6" s="119" t="s">
         <v>240</v>
       </c>
-      <c r="V6" s="112"/>
+      <c r="V6" s="108"/>
       <c r="W6" s="28" t="s">
         <v>255</v>
       </c>
@@ -16632,38 +16635,38 @@
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="118" t="s">
+      <c r="E7" s="116" t="s">
         <v>258</v>
       </c>
-      <c r="F7" s="119"/>
-      <c r="G7" s="118" t="s">
+      <c r="F7" s="117"/>
+      <c r="G7" s="116" t="s">
         <v>259</v>
       </c>
-      <c r="H7" s="119"/>
-      <c r="I7" s="118" t="s">
+      <c r="H7" s="117"/>
+      <c r="I7" s="116" t="s">
         <v>260</v>
       </c>
-      <c r="J7" s="119"/>
-      <c r="K7" s="118" t="s">
+      <c r="J7" s="117"/>
+      <c r="K7" s="116" t="s">
         <v>261</v>
       </c>
-      <c r="L7" s="119"/>
-      <c r="M7" s="117" t="s">
+      <c r="L7" s="117"/>
+      <c r="M7" s="113" t="s">
         <v>262</v>
       </c>
-      <c r="N7" s="115"/>
-      <c r="O7" s="117" t="s">
+      <c r="N7" s="114"/>
+      <c r="O7" s="113" t="s">
         <v>263</v>
       </c>
-      <c r="P7" s="115"/>
-      <c r="Q7" s="117" t="s">
+      <c r="P7" s="114"/>
+      <c r="Q7" s="113" t="s">
         <v>264</v>
       </c>
-      <c r="R7" s="115"/>
-      <c r="S7" s="117" t="s">
+      <c r="R7" s="114"/>
+      <c r="S7" s="113" t="s">
         <v>265</v>
       </c>
-      <c r="T7" s="115"/>
+      <c r="T7" s="114"/>
       <c r="U7" s="33" t="s">
         <v>266</v>
       </c>
@@ -21956,6 +21959,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="O6:P6"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="O7:P7"/>
@@ -21969,12 +21978,6 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G7:H7"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="O6:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -21986,7 +21989,8 @@
   <dimension ref="A1:S43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <pane xSplit="6760" topLeftCell="R1" activePane="topRight"/>
+      <selection pane="topRight" activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -22044,7 +22048,7 @@
         <v>282</v>
       </c>
       <c r="R1" s="90" t="s">
-        <v>257</v>
+        <v>286</v>
       </c>
       <c r="S1" s="93" t="s">
         <v>283</v>
@@ -22102,8 +22106,8 @@
       <c r="Q2" s="91">
         <v>4.5738387096774193</v>
       </c>
-      <c r="R2" s="91" t="s">
-        <v>282</v>
+      <c r="R2" s="92">
+        <v>8</v>
       </c>
       <c r="S2" s="94">
         <v>1</v>
@@ -22210,8 +22214,8 @@
       <c r="Q4" s="91">
         <v>5</v>
       </c>
-      <c r="R4" s="92">
-        <v>5</v>
+      <c r="R4" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S4" s="89"/>
     </row>
@@ -22249,8 +22253,8 @@
       <c r="Q5" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R5" s="92">
-        <v>5</v>
+      <c r="R5" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S5" s="89"/>
     </row>
@@ -22288,8 +22292,8 @@
       <c r="Q6" s="91">
         <v>5</v>
       </c>
-      <c r="R6" s="92">
-        <v>5</v>
+      <c r="R6" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S6" s="89"/>
     </row>
@@ -22345,8 +22349,8 @@
       <c r="Q7" s="91">
         <v>4.599552995391706</v>
       </c>
-      <c r="R7" s="92" t="s">
-        <v>282</v>
+      <c r="R7" s="92">
+        <v>7</v>
       </c>
       <c r="S7" s="94">
         <v>1</v>
@@ -22390,8 +22394,8 @@
       <c r="Q8" s="91">
         <v>5</v>
       </c>
-      <c r="R8" s="92">
-        <v>5</v>
+      <c r="R8" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S8" s="95"/>
     </row>
@@ -22433,8 +22437,8 @@
       <c r="Q9" s="91">
         <v>5</v>
       </c>
-      <c r="R9" s="92">
-        <v>5</v>
+      <c r="R9" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S9" s="95"/>
     </row>
@@ -22558,8 +22562,8 @@
       <c r="Q12" s="91">
         <v>5</v>
       </c>
-      <c r="R12" s="92">
-        <v>5</v>
+      <c r="R12" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S12" s="95"/>
     </row>
@@ -22597,8 +22601,8 @@
       <c r="Q13" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R13" s="92">
-        <v>5</v>
+      <c r="R13" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S13" s="95"/>
     </row>
@@ -22654,8 +22658,8 @@
       <c r="Q14" s="91">
         <v>4.3351520737327185</v>
       </c>
-      <c r="R14" s="92" t="s">
-        <v>282</v>
+      <c r="R14" s="92">
+        <v>6</v>
       </c>
       <c r="S14" s="94">
         <v>1</v>
@@ -22856,8 +22860,8 @@
       <c r="Q18" s="91">
         <v>5</v>
       </c>
-      <c r="R18" s="92">
-        <v>5</v>
+      <c r="R18" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S18" s="95"/>
     </row>
@@ -23052,8 +23056,8 @@
       <c r="Q22" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R22" s="92">
-        <v>5</v>
+      <c r="R22" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S22" s="95"/>
     </row>
@@ -23091,8 +23095,8 @@
       <c r="Q23" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R23" s="92">
-        <v>5</v>
+      <c r="R23" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S23" s="95"/>
     </row>
@@ -23207,8 +23211,8 @@
       <c r="Q25" s="91">
         <v>4.835341013824884</v>
       </c>
-      <c r="R25" s="92" t="s">
-        <v>282</v>
+      <c r="R25" s="92">
+        <v>6</v>
       </c>
       <c r="S25" s="94">
         <v>1</v>
@@ -23248,8 +23252,8 @@
       <c r="Q26" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R26" s="92">
-        <v>5</v>
+      <c r="R26" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S26" s="95"/>
     </row>
@@ -23287,8 +23291,8 @@
       <c r="Q27" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R27" s="92">
-        <v>5</v>
+      <c r="R27" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S27" s="95"/>
     </row>
@@ -23345,7 +23349,7 @@
         <v>4.8</v>
       </c>
       <c r="R28" s="92" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="S28" s="94">
         <v>1</v>
@@ -23385,8 +23389,8 @@
       <c r="Q29" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R29" s="92">
-        <v>5</v>
+      <c r="R29" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S29" s="95"/>
     </row>
@@ -23526,8 +23530,8 @@
       <c r="Q32" s="91">
         <v>5</v>
       </c>
-      <c r="R32" s="92">
-        <v>5</v>
+      <c r="R32" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S32" s="95"/>
     </row>
@@ -23612,8 +23616,8 @@
       <c r="Q34" s="91">
         <v>5</v>
       </c>
-      <c r="R34" s="92">
-        <v>5</v>
+      <c r="R34" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S34" s="95"/>
     </row>
@@ -23657,8 +23661,8 @@
       <c r="Q35" s="91">
         <v>5</v>
       </c>
-      <c r="R35" s="92">
-        <v>5</v>
+      <c r="R35" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S35" s="95"/>
     </row>
@@ -23710,8 +23714,8 @@
       <c r="Q36" s="91">
         <v>4.035783410138249</v>
       </c>
-      <c r="R36" s="92">
-        <v>5</v>
+      <c r="R36" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S36" s="95"/>
     </row>
@@ -23826,8 +23830,8 @@
       <c r="Q38" s="91">
         <v>4.564562211981567</v>
       </c>
-      <c r="R38" s="92" t="s">
-        <v>282</v>
+      <c r="R38" s="92">
+        <v>7</v>
       </c>
       <c r="S38" s="94">
         <v>1</v>
@@ -23867,8 +23871,8 @@
       <c r="Q39" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="R39" s="92">
-        <v>5</v>
+      <c r="R39" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S39" s="95"/>
     </row>
@@ -23908,8 +23912,8 @@
       <c r="Q40" s="91">
         <v>5</v>
       </c>
-      <c r="R40" s="92">
-        <v>5</v>
+      <c r="R40" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S40" s="95"/>
     </row>
@@ -23951,8 +23955,8 @@
       <c r="Q41" s="91">
         <v>5</v>
       </c>
-      <c r="R41" s="92">
-        <v>5</v>
+      <c r="R41" s="92" t="s">
+        <v>271</v>
       </c>
       <c r="S41" s="95"/>
     </row>
@@ -24048,7 +24052,7 @@
         <v>2.3573870967741932</v>
       </c>
       <c r="R43" s="92" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="S43" s="94">
         <v>1</v>
@@ -24056,5 +24060,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>